<commit_message>
gps.kml with colored pins
</commit_message>
<xml_diff>
--- a/locations.xlsx
+++ b/locations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="117">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -133,69 +133,42 @@
     <t xml:space="preserve">#</t>
   </si>
   <si>
-    <t xml:space="preserve">Blue Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cplAZ3Rblah69SQfE8js.heic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/19/2023 8:42:45 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41.7477138888889</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-87.5697222222222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8111, South Luella Avenue, South Chicago, Chicago, Hyde Park Township, Cook County, Illinois, 60617, United States</t>
+    <t xml:space="preserve">IMG_1045.JPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/15/2021 5:21:51 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41.8637888888889</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-87.8146277777778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crazy Grill Buffet, Roosevelt Road, Forest Park, Proviso Township, Cook County, Illinois, 60130, United States</t>
   </si>
   <si>
     <t xml:space="preserve">Images</t>
   </si>
   <si>
+    <t xml:space="preserve">Crazy Grill Buffet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest Park</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cook County</t>
   </si>
   <si>
     <t xml:space="preserve">IL</t>
   </si>
   <si>
-    <t xml:space="preserve">60617</t>
+    <t xml:space="preserve">60130</t>
   </si>
   <si>
     <t xml:space="preserve">US</t>
   </si>
   <si>
-    <t xml:space="preserve">41.7477138888889, -87.5697222222222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMG_1045.JPG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/15/2021 5:21:51 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41.8637888888889</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-87.8146277777778</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crazy Grill Buffet, Roosevelt Road, Forest Park, Proviso Township, Cook County, Illinois, 60130, United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crazy Grill Buffet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roosevelt Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forest Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60130</t>
-  </si>
-  <si>
     <t xml:space="preserve">12/26/2023 11:01:31 AM(UTC-6)</t>
   </si>
   <si>
@@ -286,9 +259,6 @@
     <t xml:space="preserve">14447</t>
   </si>
   <si>
-    <t xml:space="preserve">West 159th Street</t>
-  </si>
-  <si>
     <t xml:space="preserve">Homer Glen</t>
   </si>
   <si>
@@ -364,9 +334,6 @@
     <t xml:space="preserve">8701</t>
   </si>
   <si>
-    <t xml:space="preserve">Industrial Drive</t>
-  </si>
-  <si>
     <t xml:space="preserve">Justice</t>
   </si>
   <si>
@@ -376,7 +343,34 @@
     <t xml:space="preserve">No_Plate2</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">Willis Tower – Address only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">233 S Wacker Dr, Chicago, IL 60606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicago Cloud Gate Fulladdress only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedway, Loop, Chicago, Cook County, Illinois, 60602, United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201 E Randolph St, Chicago, IL 60601 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midway GPS only</t>
   </si>
 </sst>
 </file>
@@ -386,7 +380,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -408,12 +402,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -476,7 +464,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -490,10 +478,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -581,10 +565,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="B12" activeCellId="0" sqref="2:12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.96"/>
@@ -707,103 +691,100 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="U2" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="V2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AJ2" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK2" s="0" t="n">
-        <v>2</v>
+        <v>599</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="V3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="Y3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="V3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z3" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="AJ3" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK3" s="0" t="n">
-        <v>599</v>
+        <v>753</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="0" t="s">
         <v>58</v>
       </c>
@@ -813,342 +794,373 @@
       <c r="G4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="Y4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z4" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="AA4" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="V4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="X4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="AJ4" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AK4" s="0" t="n">
-        <v>753</v>
+        <v>795</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="G5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="V5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="Y5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z5" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="V5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="X5" s="0" t="s">
+      <c r="AA5" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="Y5" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="AJ5" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AK5" s="0" t="n">
-        <v>795</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>71</v>
+      </c>
       <c r="B6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="I6" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="J6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z6" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="V6" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="W6" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y6" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z6" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA6" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="AJ6" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AK6" s="0" t="n">
-        <v>1607</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="I7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="R7" s="0" t="s">
+      <c r="V7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA7" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="S7" s="0" t="s">
+      <c r="AB7" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="T7" s="0" t="s">
+      <c r="AG7" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="U7" s="0" t="s">
+      <c r="AH7" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="V7" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="X7" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z7" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="AJ7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="AK7" s="0" t="n">
-        <v>1766</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="I8" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="J8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="0" t="s">
         <v>95</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB8" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="AG8" s="4" t="s">
+      <c r="AG8" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="AH8" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="AJ8" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="J9" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="S9" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="U9" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="V9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA9" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="V9" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="W9" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="X9" s="0" t="s">
+      <c r="AB9" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="Y9" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z9" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA9" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="AG9" s="0" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="AJ9" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="0" t="s">
+      <c r="J11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="U11" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="V11" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="O10" s="0" t="s">
+      <c r="W11" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="S10" s="0" t="s">
+      <c r="X11" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="T10" s="0" t="s">
+      <c r="Y11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z11" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="U10" s="0" t="s">
+      <c r="AA11" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="V10" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="W10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="X10" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y10" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z10" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA10" s="0" t="s">
+      <c r="AJ11" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="AB10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG10" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ10" s="0" t="n">
-        <v>10</v>
+      <c r="F12" s="0" t="n">
+        <v>41.7854316</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>-87.7508486935715</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ12" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="0" t="s">
-        <v>118</v>
-      </c>
-    </row>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>